<commit_message>
updated Master_vars, reorganized folders
</commit_message>
<xml_diff>
--- a/master_vars.xlsx
+++ b/master_vars.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18023" windowHeight="5213"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18020" windowHeight="5210"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="287">
   <si>
     <t>Housing Age</t>
   </si>
@@ -1002,26 +1002,11 @@
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1036,9 +1021,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1052,6 +1034,24 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1336,1688 +1336,1763 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.46484375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="35.19921875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="24.46484375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="48.53125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="35.1796875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="24.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="48.54296875" style="1" customWidth="1"/>
     <col min="6" max="6" width="39" style="1" customWidth="1"/>
-    <col min="7" max="7" width="24.53125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="32.19921875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="46.33203125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.73046875" style="1"/>
+    <col min="7" max="7" width="24.54296875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="32.1796875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="46.36328125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="15" t="s">
         <v>283</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="15" t="s">
         <v>285</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="13" t="s">
         <v>282</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="13" t="s">
         <v>281</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="13" t="s">
         <v>276</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="13" t="s">
         <v>277</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="13" t="s">
         <v>278</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="I1" s="13" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A3" s="2"/>
-      <c r="B3" s="10" t="s">
+      <c r="I2" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="17"/>
+      <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="11" t="s">
+      <c r="D3" s="17"/>
+      <c r="E3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2" t="s">
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="17"/>
+      <c r="B4" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="11" t="s">
+      <c r="D4" s="17"/>
+      <c r="E4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="11" t="s">
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="17"/>
+      <c r="E5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2" t="s">
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="17"/>
+      <c r="B6" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="11" t="s">
+      <c r="D6" s="17"/>
+      <c r="E6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="11" t="s">
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="17"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="17"/>
+      <c r="E7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="10" t="s">
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="5" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="11" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="17"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="17"/>
+      <c r="E8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="10" t="s">
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="5" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="17"/>
+      <c r="B9" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="11" t="s">
+      <c r="D9" s="17"/>
+      <c r="E9" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="10" t="s">
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="5" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="11" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="17"/>
+      <c r="E10" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A11" s="2" t="s">
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="10" t="s">
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="5" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="11" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="17"/>
+      <c r="E12" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="10" t="s">
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="17"/>
+      <c r="B13" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="11" t="s">
+      <c r="D13" s="17"/>
+      <c r="E13" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="11" t="s">
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="17"/>
+      <c r="E14" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="11" t="s">
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="17"/>
+      <c r="E15" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="F15" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2" t="s">
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="17"/>
+      <c r="B16" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="11" t="s">
+      <c r="D16" s="17"/>
+      <c r="E16" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="11" t="s">
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="17"/>
+      <c r="E17" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F17" s="12" t="s">
+      <c r="F17" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="11" t="s">
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A18" s="17"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="17"/>
+      <c r="E18" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F18" s="12" t="s">
+      <c r="F18" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A19" s="4" t="s">
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A19" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="F19" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="G19" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="H19" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="I19" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A20" s="4"/>
-      <c r="B20" s="7" t="s">
+      <c r="I19" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A20" s="16"/>
+      <c r="B20" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="6" t="s">
+      <c r="D20" s="19"/>
+      <c r="E20" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F20" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A21" s="4"/>
-      <c r="B21" s="7" t="s">
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A21" s="16"/>
+      <c r="B21" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="6" t="s">
+      <c r="D21" s="19"/>
+      <c r="E21" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="F21" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="10" t="s">
-        <v>244</v>
-      </c>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A22" s="4"/>
-      <c r="B22" s="7" t="s">
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A22" s="16"/>
+      <c r="B22" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="6" t="s">
+      <c r="D22" s="20"/>
+      <c r="E22" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="10" t="s">
-        <v>244</v>
-      </c>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="3"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A23" s="2" t="s">
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="2"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A23" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="16" t="s">
         <v>73</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E23" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F23" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="G23" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="H23" s="4" t="s">
+      <c r="H23" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="I23" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A24" s="2"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="6" t="s">
+      <c r="I23" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A24" s="17"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" s="19"/>
+      <c r="E24" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="F24" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A25" s="2"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="6" t="s">
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A25" s="17"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" s="19"/>
+      <c r="E25" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="F25" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A26" s="2"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="6" t="s">
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A26" s="17"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" s="19"/>
+      <c r="E26" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="F26" s="7" t="s">
+      <c r="F26" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A27" s="2"/>
-      <c r="B27" s="4" t="s">
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A27" s="17"/>
+      <c r="B27" s="16" t="s">
         <v>85</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D27" s="8"/>
-      <c r="E27" s="6" t="s">
+      <c r="D27" s="19"/>
+      <c r="E27" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="F27" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A28" s="2"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="6" t="s">
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A28" s="17"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D28" s="19"/>
+      <c r="E28" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="F28" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A29" s="2"/>
-      <c r="B29" s="4" t="s">
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A29" s="17"/>
+      <c r="B29" s="16" t="s">
         <v>91</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D29" s="8"/>
-      <c r="E29" s="6" t="s">
+      <c r="D29" s="19"/>
+      <c r="E29" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="F29" s="7" t="s">
+      <c r="F29" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A30" s="2"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="6" t="s">
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A30" s="17"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D30" s="19"/>
+      <c r="E30" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="F30" s="7" t="s">
+      <c r="F30" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A31" s="2"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="6" t="s">
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A31" s="17"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D31" s="19"/>
+      <c r="E31" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="F31" s="7" t="s">
+      <c r="F31" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A32" s="2"/>
-      <c r="B32" s="4" t="s">
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A32" s="17"/>
+      <c r="B32" s="16" t="s">
         <v>99</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="D32" s="8"/>
-      <c r="E32" s="6" t="s">
+      <c r="D32" s="19"/>
+      <c r="E32" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="F32" s="7" t="s">
+      <c r="F32" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A33" s="2"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="6" t="s">
+      <c r="G32" s="16"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A33" s="17"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D33" s="19"/>
+      <c r="E33" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="F33" s="7" t="s">
+      <c r="F33" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A34" s="2"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="6" t="s">
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A34" s="17"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D34" s="20"/>
+      <c r="E34" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="F34" s="7" t="s">
+      <c r="F34" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A35" s="2" t="s">
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A35" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C35" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="E35" s="6" t="s">
+      <c r="E35" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="F35" s="12" t="s">
+      <c r="F35" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="G35" s="4" t="s">
+      <c r="G35" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="H35" s="14" t="s">
+      <c r="H35" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="I35" s="17" t="s">
+      <c r="I35" s="11" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A36" s="2"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="7" t="s">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A36" s="17"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D36" s="8"/>
-      <c r="E36" s="6" t="s">
+      <c r="D36" s="19"/>
+      <c r="E36" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="F36" s="12" t="s">
+      <c r="F36" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="G36" s="4"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="17" t="s">
+      <c r="G36" s="16"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="11" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A37" s="2"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="7" t="s">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A37" s="17"/>
+      <c r="B37" s="16"/>
+      <c r="C37" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D37" s="8"/>
-      <c r="E37" s="6" t="s">
+      <c r="D37" s="19"/>
+      <c r="E37" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="F37" s="12" t="s">
+      <c r="F37" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="G37" s="4"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="17" t="s">
+      <c r="G37" s="16"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="11" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A38" s="2"/>
-      <c r="B38" s="7" t="s">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A38" s="17"/>
+      <c r="B38" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="C38" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D38" s="8"/>
-      <c r="E38" s="6" t="s">
+      <c r="D38" s="19"/>
+      <c r="E38" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="F38" s="12" t="s">
+      <c r="F38" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="G38" s="4"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="17" t="s">
+      <c r="G38" s="16"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="11" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A39" s="2"/>
-      <c r="B39" s="4" t="s">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A39" s="17"/>
+      <c r="B39" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="C39" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="D39" s="8"/>
-      <c r="E39" s="6" t="s">
+      <c r="D39" s="19"/>
+      <c r="E39" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="F39" s="12" t="s">
+      <c r="F39" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="G39" s="4"/>
-      <c r="H39" s="14"/>
-      <c r="I39" s="17" t="s">
+      <c r="G39" s="16"/>
+      <c r="H39" s="21"/>
+      <c r="I39" s="11" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A40" s="2"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="7" t="s">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A40" s="17"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="D40" s="9"/>
-      <c r="E40" s="6" t="s">
+      <c r="D40" s="20"/>
+      <c r="E40" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="F40" s="12" t="s">
+      <c r="F40" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="G40" s="4"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="17" t="s">
+      <c r="G40" s="16"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="11" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A41" s="4" t="s">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A41" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="B41" s="15" t="s">
+      <c r="B41" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="C41" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D41" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E41" s="15" t="s">
+      <c r="E41" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="F41" s="15" t="s">
+      <c r="F41" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="G41" s="5" t="s">
+      <c r="G41" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="H41" s="5" t="s">
+      <c r="H41" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="I41" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A42" s="4"/>
-      <c r="B42" s="15" t="s">
+      <c r="I41" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A42" s="16"/>
+      <c r="B42" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="C42" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D42" s="8"/>
-      <c r="E42" s="15" t="s">
+      <c r="D42" s="19"/>
+      <c r="E42" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="F42" s="15" t="s">
+      <c r="F42" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="G42" s="8"/>
-      <c r="H42" s="8"/>
-      <c r="I42" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A43" s="4"/>
-      <c r="B43" s="15" t="s">
+      <c r="G42" s="19"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A43" s="16"/>
+      <c r="B43" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="C43" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="D43" s="8"/>
-      <c r="E43" s="15" t="s">
+      <c r="D43" s="19"/>
+      <c r="E43" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="F43" s="15" t="s">
+      <c r="F43" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="G43" s="8"/>
-      <c r="H43" s="8"/>
-      <c r="I43" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="21.7" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="4"/>
-      <c r="B44" s="15" t="s">
+      <c r="G43" s="19"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="16"/>
+      <c r="B44" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="C44" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="D44" s="9"/>
-      <c r="E44" s="15" t="s">
+      <c r="D44" s="20"/>
+      <c r="E44" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F44" s="15" t="s">
+      <c r="F44" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="G44" s="9"/>
-      <c r="H44" s="9"/>
-      <c r="I44" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="2" t="s">
+      <c r="G44" s="20"/>
+      <c r="H44" s="20"/>
+      <c r="I44" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="16" t="s">
         <v>146</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D45" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E45" s="15" t="s">
+      <c r="E45" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="F45" s="15" t="s">
+      <c r="F45" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="G45" s="5" t="s">
+      <c r="G45" s="18" t="s">
         <v>279</v>
       </c>
-      <c r="H45" s="5" t="s">
+      <c r="H45" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="I45" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="2"/>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="15" t="s">
+      <c r="I45" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="17"/>
+      <c r="B46" s="16"/>
+      <c r="C46" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D46" s="19"/>
+      <c r="E46" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="F46" s="15" t="s">
+      <c r="F46" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="G46" s="8"/>
-      <c r="H46" s="8"/>
-      <c r="I46" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="2"/>
-      <c r="B47" s="4" t="s">
+      <c r="G46" s="19"/>
+      <c r="H46" s="19"/>
+      <c r="I46" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="17"/>
+      <c r="B47" s="16" t="s">
         <v>153</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="D47" s="8"/>
-      <c r="E47" s="15" t="s">
+      <c r="D47" s="19"/>
+      <c r="E47" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="F47" s="15" t="s">
+      <c r="F47" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="G47" s="8"/>
-      <c r="H47" s="8"/>
-      <c r="I47" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="2"/>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="15" t="s">
+      <c r="G47" s="19"/>
+      <c r="H47" s="19"/>
+      <c r="I47" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="17"/>
+      <c r="B48" s="16"/>
+      <c r="C48" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D48" s="19"/>
+      <c r="E48" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="F48" s="15" t="s">
+      <c r="F48" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="G48" s="8"/>
-      <c r="H48" s="8"/>
-      <c r="I48" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="2"/>
-      <c r="B49" s="4" t="s">
+      <c r="G48" s="19"/>
+      <c r="H48" s="19"/>
+      <c r="I48" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="17"/>
+      <c r="B49" s="16" t="s">
         <v>159</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="D49" s="8"/>
-      <c r="E49" s="15" t="s">
+      <c r="D49" s="19"/>
+      <c r="E49" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="F49" s="15" t="s">
+      <c r="F49" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="G49" s="8"/>
-      <c r="H49" s="8"/>
-      <c r="I49" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="2"/>
-      <c r="B50" s="4"/>
-      <c r="C50" s="4"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="15" t="s">
+      <c r="G49" s="19"/>
+      <c r="H49" s="19"/>
+      <c r="I49" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="17"/>
+      <c r="B50" s="16"/>
+      <c r="C50" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="D50" s="19"/>
+      <c r="E50" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="F50" s="15" t="s">
+      <c r="F50" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="G50" s="8"/>
-      <c r="H50" s="8"/>
-      <c r="I50" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="2"/>
-      <c r="B51" s="4" t="s">
+      <c r="G50" s="19"/>
+      <c r="H50" s="19"/>
+      <c r="I50" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="17"/>
+      <c r="B51" s="16" t="s">
         <v>165</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="D51" s="8"/>
-      <c r="E51" s="15" t="s">
+      <c r="D51" s="19"/>
+      <c r="E51" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="F51" s="15" t="s">
+      <c r="F51" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="G51" s="8"/>
-      <c r="H51" s="8"/>
-      <c r="I51" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A52" s="2"/>
-      <c r="B52" s="4"/>
-      <c r="C52" s="4"/>
-      <c r="D52" s="8"/>
-      <c r="E52" s="15" t="s">
+      <c r="G51" s="19"/>
+      <c r="H51" s="19"/>
+      <c r="I51" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="17"/>
+      <c r="B52" s="16"/>
+      <c r="C52" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D52" s="19"/>
+      <c r="E52" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="F52" s="15" t="s">
+      <c r="F52" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="G52" s="8"/>
-      <c r="H52" s="8"/>
-      <c r="I52" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A53" s="2"/>
-      <c r="B53" s="4"/>
-      <c r="C53" s="4"/>
-      <c r="D53" s="8"/>
-      <c r="E53" s="15" t="s">
+      <c r="G52" s="19"/>
+      <c r="H52" s="19"/>
+      <c r="I52" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="17"/>
+      <c r="B53" s="16"/>
+      <c r="C53" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D53" s="19"/>
+      <c r="E53" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="F53" s="15" t="s">
+      <c r="F53" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="G53" s="8"/>
-      <c r="H53" s="8"/>
-      <c r="I53" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A54" s="2"/>
-      <c r="B54" s="4"/>
-      <c r="C54" s="4"/>
-      <c r="D54" s="8"/>
-      <c r="E54" s="15" t="s">
+      <c r="G53" s="19"/>
+      <c r="H53" s="19"/>
+      <c r="I53" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="17"/>
+      <c r="B54" s="16"/>
+      <c r="C54" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D54" s="19"/>
+      <c r="E54" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="F54" s="15" t="s">
+      <c r="F54" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="G54" s="8"/>
-      <c r="H54" s="8"/>
-      <c r="I54" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A55" s="2"/>
-      <c r="B55" s="4"/>
-      <c r="C55" s="4"/>
-      <c r="D55" s="8"/>
-      <c r="E55" s="15" t="s">
+      <c r="G54" s="19"/>
+      <c r="H54" s="19"/>
+      <c r="I54" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="17"/>
+      <c r="B55" s="16"/>
+      <c r="C55" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D55" s="19"/>
+      <c r="E55" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="F55" s="15" t="s">
+      <c r="F55" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="G55" s="8"/>
-      <c r="H55" s="8"/>
-      <c r="I55" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A56" s="2"/>
-      <c r="B56" s="4"/>
-      <c r="C56" s="4"/>
-      <c r="D56" s="9"/>
-      <c r="E56" s="15" t="s">
+      <c r="G55" s="19"/>
+      <c r="H55" s="19"/>
+      <c r="I55" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="17"/>
+      <c r="B56" s="16"/>
+      <c r="C56" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D56" s="20"/>
+      <c r="E56" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="F56" s="15" t="s">
+      <c r="F56" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="G56" s="9"/>
-      <c r="H56" s="9"/>
-      <c r="I56" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A57" s="10" t="s">
+      <c r="G56" s="20"/>
+      <c r="H56" s="20"/>
+      <c r="I56" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A57" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="B57" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="C57" s="7" t="s">
+      <c r="C57" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="D57" s="7" t="s">
+      <c r="D57" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E57" s="7" t="s">
+      <c r="E57" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="F57" s="7" t="s">
+      <c r="F57" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="G57" s="7" t="s">
+      <c r="G57" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="H57" s="7" t="s">
+      <c r="H57" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="I57" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A58" s="4" t="s">
+      <c r="I57" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A58" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B58" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C58" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D58" s="2" t="s">
+      <c r="D58" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E58" s="16" t="s">
+      <c r="E58" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="F58" s="16" t="s">
+      <c r="F58" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="G58" s="2" t="s">
+      <c r="G58" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="H58" s="2" t="s">
+      <c r="H58" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="I58" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A59" s="4"/>
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
-      <c r="E59" s="16" t="s">
+      <c r="I58" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A59" s="16"/>
+      <c r="B59" s="17"/>
+      <c r="C59" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D59" s="17"/>
+      <c r="E59" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="F59" s="16" t="s">
+      <c r="F59" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="G59" s="2"/>
-      <c r="H59" s="2"/>
-      <c r="I59" s="18" t="s">
+      <c r="G59" s="17"/>
+      <c r="H59" s="17"/>
+      <c r="I59" s="12" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A60" s="4"/>
-      <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
-      <c r="D60" s="2"/>
-      <c r="E60" s="16" t="s">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A60" s="16"/>
+      <c r="B60" s="17"/>
+      <c r="C60" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D60" s="17"/>
+      <c r="E60" s="10" t="s">
         <v>194</v>
       </c>
-      <c r="F60" s="16" t="s">
+      <c r="F60" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="G60" s="2"/>
-      <c r="H60" s="2"/>
-      <c r="I60" s="18" t="s">
+      <c r="G60" s="17"/>
+      <c r="H60" s="17"/>
+      <c r="I60" s="12" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A61" s="4"/>
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
-      <c r="E61" s="16" t="s">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A61" s="16"/>
+      <c r="B61" s="17"/>
+      <c r="C61" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D61" s="17"/>
+      <c r="E61" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="F61" s="16" t="s">
+      <c r="F61" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="G61" s="2"/>
-      <c r="H61" s="2"/>
-      <c r="I61" s="18" t="s">
+      <c r="G61" s="17"/>
+      <c r="H61" s="17"/>
+      <c r="I61" s="12" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A62" s="4"/>
-      <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
-      <c r="D62" s="2"/>
-      <c r="E62" s="16" t="s">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A62" s="16"/>
+      <c r="B62" s="17"/>
+      <c r="C62" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D62" s="17"/>
+      <c r="E62" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="F62" s="16" t="s">
+      <c r="F62" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="G62" s="2"/>
-      <c r="H62" s="2"/>
-      <c r="I62" s="18" t="s">
+      <c r="G62" s="17"/>
+      <c r="H62" s="17"/>
+      <c r="I62" s="12" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A63" s="4"/>
-      <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
-      <c r="D63" s="2"/>
-      <c r="E63" s="16" t="s">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A63" s="16"/>
+      <c r="B63" s="17"/>
+      <c r="C63" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D63" s="17"/>
+      <c r="E63" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="F63" s="16" t="s">
+      <c r="F63" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="G63" s="2"/>
-      <c r="H63" s="2"/>
-      <c r="I63" s="18" t="s">
+      <c r="G63" s="17"/>
+      <c r="H63" s="17"/>
+      <c r="I63" s="12" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A64" s="4"/>
-      <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
-      <c r="D64" s="2"/>
-      <c r="E64" s="16" t="s">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A64" s="16"/>
+      <c r="B64" s="17"/>
+      <c r="C64" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D64" s="17"/>
+      <c r="E64" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="F64" s="16" t="s">
+      <c r="F64" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="G64" s="2"/>
-      <c r="H64" s="2"/>
-      <c r="I64" s="18" t="s">
+      <c r="G64" s="17"/>
+      <c r="H64" s="17"/>
+      <c r="I64" s="12" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A65" s="4"/>
-      <c r="B65" s="2"/>
-      <c r="C65" s="2"/>
-      <c r="D65" s="2"/>
-      <c r="E65" s="16" t="s">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A65" s="16"/>
+      <c r="B65" s="17"/>
+      <c r="C65" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D65" s="17"/>
+      <c r="E65" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="F65" s="16" t="s">
+      <c r="F65" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="G65" s="2"/>
-      <c r="H65" s="2"/>
-      <c r="I65" s="18" t="s">
+      <c r="G65" s="17"/>
+      <c r="H65" s="17"/>
+      <c r="I65" s="12" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A66" s="4"/>
-      <c r="B66" s="2"/>
-      <c r="C66" s="2"/>
-      <c r="D66" s="2"/>
-      <c r="E66" s="16" t="s">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A66" s="16"/>
+      <c r="B66" s="17"/>
+      <c r="C66" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D66" s="17"/>
+      <c r="E66" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="F66" s="16" t="s">
+      <c r="F66" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="G66" s="2"/>
-      <c r="H66" s="2"/>
-      <c r="I66" s="18" t="s">
+      <c r="G66" s="17"/>
+      <c r="H66" s="17"/>
+      <c r="I66" s="12" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A67" s="4"/>
-      <c r="B67" s="2"/>
-      <c r="C67" s="2"/>
-      <c r="D67" s="2"/>
-      <c r="E67" s="16" t="s">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A67" s="16"/>
+      <c r="B67" s="17"/>
+      <c r="C67" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D67" s="17"/>
+      <c r="E67" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="F67" s="16" t="s">
+      <c r="F67" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="G67" s="2"/>
-      <c r="H67" s="2"/>
-      <c r="I67" s="18" t="s">
+      <c r="G67" s="17"/>
+      <c r="H67" s="17"/>
+      <c r="I67" s="12" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A68" s="4"/>
-      <c r="B68" s="2"/>
-      <c r="C68" s="2"/>
-      <c r="D68" s="2"/>
-      <c r="E68" s="16" t="s">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A68" s="16"/>
+      <c r="B68" s="17"/>
+      <c r="C68" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D68" s="17"/>
+      <c r="E68" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="F68" s="16" t="s">
+      <c r="F68" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="G68" s="2"/>
-      <c r="H68" s="2"/>
-      <c r="I68" s="18" t="s">
+      <c r="G68" s="17"/>
+      <c r="H68" s="17"/>
+      <c r="I68" s="12" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A69" s="4"/>
-      <c r="B69" s="2"/>
-      <c r="C69" s="2"/>
-      <c r="D69" s="2"/>
-      <c r="E69" s="16" t="s">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A69" s="16"/>
+      <c r="B69" s="17"/>
+      <c r="C69" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D69" s="17"/>
+      <c r="E69" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="F69" s="16" t="s">
+      <c r="F69" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="G69" s="2"/>
-      <c r="H69" s="2"/>
-      <c r="I69" s="18" t="s">
+      <c r="G69" s="17"/>
+      <c r="H69" s="17"/>
+      <c r="I69" s="12" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A70" s="4"/>
-      <c r="B70" s="2"/>
-      <c r="C70" s="2"/>
-      <c r="D70" s="2"/>
-      <c r="E70" s="16" t="s">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A70" s="16"/>
+      <c r="B70" s="17"/>
+      <c r="C70" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D70" s="17"/>
+      <c r="E70" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="F70" s="16" t="s">
+      <c r="F70" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="G70" s="2"/>
-      <c r="H70" s="2"/>
-      <c r="I70" s="18" t="s">
+      <c r="G70" s="17"/>
+      <c r="H70" s="17"/>
+      <c r="I70" s="12" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A71" s="4"/>
-      <c r="B71" s="2"/>
-      <c r="C71" s="2"/>
-      <c r="D71" s="2"/>
-      <c r="E71" s="16" t="s">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A71" s="16"/>
+      <c r="B71" s="17"/>
+      <c r="C71" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D71" s="17"/>
+      <c r="E71" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="F71" s="16" t="s">
+      <c r="F71" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="G71" s="2"/>
-      <c r="H71" s="2"/>
-      <c r="I71" s="18" t="s">
+      <c r="G71" s="17"/>
+      <c r="H71" s="17"/>
+      <c r="I71" s="12" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A72" s="4"/>
-      <c r="B72" s="2"/>
-      <c r="C72" s="2"/>
-      <c r="D72" s="2"/>
-      <c r="E72" s="16" t="s">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A72" s="16"/>
+      <c r="B72" s="17"/>
+      <c r="C72" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D72" s="17"/>
+      <c r="E72" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="F72" s="16" t="s">
+      <c r="F72" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="G72" s="2"/>
-      <c r="H72" s="2"/>
-      <c r="I72" s="18" t="s">
+      <c r="G72" s="17"/>
+      <c r="H72" s="17"/>
+      <c r="I72" s="12" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A73" s="4"/>
-      <c r="B73" s="2"/>
-      <c r="C73" s="2"/>
-      <c r="D73" s="2"/>
-      <c r="E73" s="16" t="s">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A73" s="16"/>
+      <c r="B73" s="17"/>
+      <c r="C73" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D73" s="17"/>
+      <c r="E73" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="F73" s="16" t="s">
+      <c r="F73" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="G73" s="2"/>
-      <c r="H73" s="2"/>
-      <c r="I73" s="18" t="s">
+      <c r="G73" s="17"/>
+      <c r="H73" s="17"/>
+      <c r="I73" s="12" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A74" s="4"/>
-      <c r="B74" s="2"/>
-      <c r="C74" s="2"/>
-      <c r="D74" s="2"/>
-      <c r="E74" s="16" t="s">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A74" s="16"/>
+      <c r="B74" s="17"/>
+      <c r="C74" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D74" s="17"/>
+      <c r="E74" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="F74" s="16" t="s">
+      <c r="F74" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="G74" s="2"/>
-      <c r="H74" s="2"/>
-      <c r="I74" s="18" t="s">
+      <c r="G74" s="17"/>
+      <c r="H74" s="17"/>
+      <c r="I74" s="12" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A75" s="4"/>
-      <c r="B75" s="2" t="s">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A75" s="16"/>
+      <c r="B75" s="17" t="s">
         <v>224</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="C75" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="D75" s="2"/>
-      <c r="E75" s="16" t="s">
+      <c r="D75" s="17"/>
+      <c r="E75" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="F75" s="16" t="s">
+      <c r="F75" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="G75" s="2"/>
-      <c r="H75" s="2"/>
-      <c r="I75" s="18" t="s">
+      <c r="G75" s="17"/>
+      <c r="H75" s="17"/>
+      <c r="I75" s="12" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A76" s="4"/>
-      <c r="B76" s="2"/>
-      <c r="C76" s="2"/>
-      <c r="D76" s="2"/>
-      <c r="E76" s="16" t="s">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A76" s="16"/>
+      <c r="B76" s="17"/>
+      <c r="C76" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="D76" s="17"/>
+      <c r="E76" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="F76" s="16" t="s">
+      <c r="F76" s="10" t="s">
         <v>229</v>
       </c>
-      <c r="G76" s="2"/>
-      <c r="H76" s="2"/>
-      <c r="I76" s="18" t="s">
+      <c r="G76" s="17"/>
+      <c r="H76" s="17"/>
+      <c r="I76" s="12" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A77" s="4"/>
-      <c r="B77" s="2"/>
-      <c r="C77" s="2"/>
-      <c r="D77" s="2"/>
-      <c r="E77" s="16" t="s">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A77" s="16"/>
+      <c r="B77" s="17"/>
+      <c r="C77" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="D77" s="17"/>
+      <c r="E77" s="10" t="s">
         <v>230</v>
       </c>
-      <c r="F77" s="16" t="s">
+      <c r="F77" s="10" t="s">
         <v>231</v>
       </c>
-      <c r="G77" s="2"/>
-      <c r="H77" s="2"/>
-      <c r="I77" s="18" t="s">
+      <c r="G77" s="17"/>
+      <c r="H77" s="17"/>
+      <c r="I77" s="12" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A78" s="4"/>
-      <c r="B78" s="2"/>
-      <c r="C78" s="2"/>
-      <c r="D78" s="2"/>
-      <c r="E78" s="16" t="s">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A78" s="16"/>
+      <c r="B78" s="17"/>
+      <c r="C78" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="D78" s="17"/>
+      <c r="E78" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="F78" s="16" t="s">
+      <c r="F78" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="G78" s="2"/>
-      <c r="H78" s="2"/>
-      <c r="I78" s="18" t="s">
+      <c r="G78" s="17"/>
+      <c r="H78" s="17"/>
+      <c r="I78" s="12" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A79" s="4"/>
-      <c r="B79" s="2" t="s">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A79" s="16"/>
+      <c r="B79" s="17" t="s">
         <v>234</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="C79" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="D79" s="2"/>
-      <c r="E79" s="16" t="s">
+      <c r="D79" s="17"/>
+      <c r="E79" s="10" t="s">
         <v>236</v>
       </c>
-      <c r="F79" s="16" t="s">
+      <c r="F79" s="10" t="s">
         <v>237</v>
       </c>
-      <c r="G79" s="2"/>
-      <c r="H79" s="2"/>
-      <c r="I79" s="18" t="s">
+      <c r="G79" s="17"/>
+      <c r="H79" s="17"/>
+      <c r="I79" s="12" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A80" s="4"/>
-      <c r="B80" s="2"/>
-      <c r="C80" s="2"/>
-      <c r="D80" s="2"/>
-      <c r="E80" s="16" t="s">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A80" s="16"/>
+      <c r="B80" s="17"/>
+      <c r="C80" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="D80" s="17"/>
+      <c r="E80" s="10" t="s">
         <v>238</v>
       </c>
-      <c r="F80" s="16" t="s">
+      <c r="F80" s="10" t="s">
         <v>239</v>
       </c>
-      <c r="G80" s="2"/>
-      <c r="H80" s="2"/>
-      <c r="I80" s="18" t="s">
+      <c r="G80" s="17"/>
+      <c r="H80" s="17"/>
+      <c r="I80" s="12" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A81" s="4"/>
-      <c r="B81" s="2"/>
-      <c r="C81" s="2"/>
-      <c r="D81" s="2"/>
-      <c r="E81" s="16" t="s">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A81" s="16"/>
+      <c r="B81" s="17"/>
+      <c r="C81" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="D81" s="17"/>
+      <c r="E81" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="F81" s="16" t="s">
+      <c r="F81" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="G81" s="2"/>
-      <c r="H81" s="2"/>
-      <c r="I81" s="18" t="s">
+      <c r="G81" s="17"/>
+      <c r="H81" s="17"/>
+      <c r="I81" s="12" t="s">
         <v>275</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="66">
-    <mergeCell ref="A58:A81"/>
-    <mergeCell ref="B58:B74"/>
-    <mergeCell ref="C58:C74"/>
-    <mergeCell ref="D58:D81"/>
-    <mergeCell ref="G58:G81"/>
-    <mergeCell ref="H58:H81"/>
-    <mergeCell ref="B75:B78"/>
-    <mergeCell ref="C75:C78"/>
-    <mergeCell ref="B79:B81"/>
-    <mergeCell ref="C79:C81"/>
+  <mergeCells count="49">
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="D2:D10"/>
+    <mergeCell ref="G2:G18"/>
+    <mergeCell ref="H2:H18"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="A11:A18"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="D11:D18"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="G19:G22"/>
+    <mergeCell ref="H19:H22"/>
+    <mergeCell ref="A23:A34"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="D23:D34"/>
+    <mergeCell ref="G23:G34"/>
+    <mergeCell ref="H23:H34"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="A35:A40"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="D35:D40"/>
+    <mergeCell ref="G35:G40"/>
+    <mergeCell ref="H35:H40"/>
+    <mergeCell ref="B39:B40"/>
     <mergeCell ref="A41:A44"/>
     <mergeCell ref="D41:D44"/>
     <mergeCell ref="G41:G44"/>
     <mergeCell ref="H41:H44"/>
     <mergeCell ref="A45:A56"/>
     <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
     <mergeCell ref="D45:D56"/>
     <mergeCell ref="G45:G56"/>
     <mergeCell ref="H45:H56"/>
     <mergeCell ref="B47:B48"/>
-    <mergeCell ref="C47:C48"/>
     <mergeCell ref="B49:B50"/>
-    <mergeCell ref="C49:C50"/>
     <mergeCell ref="B51:B56"/>
-    <mergeCell ref="C51:C56"/>
-    <mergeCell ref="A35:A40"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="D35:D40"/>
-    <mergeCell ref="G35:G40"/>
-    <mergeCell ref="H35:H40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="H19:H22"/>
-    <mergeCell ref="A23:A34"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="C23:C26"/>
-    <mergeCell ref="D23:D34"/>
-    <mergeCell ref="G23:G34"/>
-    <mergeCell ref="H23:H34"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="G19:G22"/>
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="D2:D10"/>
-    <mergeCell ref="G2:G18"/>
-    <mergeCell ref="H2:H18"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="A11:A18"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D18"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="H58:H81"/>
+    <mergeCell ref="B75:B78"/>
+    <mergeCell ref="B79:B81"/>
+    <mergeCell ref="A58:A81"/>
+    <mergeCell ref="B58:B74"/>
+    <mergeCell ref="D58:D81"/>
+    <mergeCell ref="G58:G81"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>